<commit_message>
update export.controller.js, exported_companys.xlsx and imports.controller.js
</commit_message>
<xml_diff>
--- a/src/main/export/exported_companys.xlsx
+++ b/src/main/export/exported_companys.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>brand_label</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>brand_image</t>
-  </si>
-  <si>
-    <t>brand_slug</t>
   </si>
   <si>
     <t>brand_description</t>
@@ -441,7 +438,7 @@
   <dimension ref="A1:F3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,46 +453,43 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update export.controller.js and exported_companys.xlsx
</commit_message>
<xml_diff>
--- a/src/main/export/exported_companys.xlsx
+++ b/src/main/export/exported_companys.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>brand_label</t>
   </si>
@@ -40,9 +40,6 @@
     <t>https://rest.app.gobd.xyz/uploads/e580bcff-6368-4b4c-822f-fe14822b4553.png</t>
   </si>
   <si>
-    <t>wayback</t>
-  </si>
-  <si>
     <t>United States of America NSA</t>
   </si>
   <si>
@@ -58,7 +55,7 @@
     <t>https://rest.app.gobd.xyz/uploads/d0fbcd9e-9a78-4d23-8721-2b711b67ab49.jpg</t>
   </si>
   <si>
-    <t>demo-company</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -435,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -455,7 +452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -470,26 +467,40 @@
       </c>
       <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>